<commit_message>
added data, updated scripts
</commit_message>
<xml_diff>
--- a/conservation_latest_data/conservation_summary.xlsx
+++ b/conservation_latest_data/conservation_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="249" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="249" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="397">
   <si>
     <t>Gene</t>
   </si>
@@ -976,6 +976,24 @@
   </si>
   <si>
     <t>p value</t>
+  </si>
+  <si>
+    <t>JS &amp; JS p</t>
+  </si>
+  <si>
+    <t>JSP &amp; JSP p</t>
+  </si>
+  <si>
+    <t>SE &amp; SE p</t>
+  </si>
+  <si>
+    <t>SEP &amp; SEP p</t>
+  </si>
+  <si>
+    <t>SoP &amp; SoP p</t>
+  </si>
+  <si>
+    <t>SoPP &amp; SoPP p</t>
   </si>
   <si>
     <t>procollagen-lysine 5-dioxygenase activity</t>
@@ -1342,7 +1360,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1358,7 +1376,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF008000"/>
-        <bgColor rgb="FF006411"/>
+        <bgColor rgb="FF009900"/>
       </patternFill>
     </fill>
     <fill>
@@ -1389,6 +1407,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009900"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1477,7 +1501,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1926,6 +1950,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1950,7 +1978,7 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF009900"/>
       <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -2005,7 +2033,7 @@
   </sheetPr>
   <dimension ref="A1:AH264"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
@@ -28067,10 +28095,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L254"/>
+  <dimension ref="A1:AB254"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -28106,15 +28134,73 @@
       <c r="G1" s="110" t="s">
         <v>319</v>
       </c>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="110"/>
+      <c r="H1" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="110" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="110" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="110" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="110" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="110" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="110" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="110" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="110" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="110" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="110" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="110" t="s">
+        <v>320</v>
+      </c>
+      <c r="X1" s="110" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y1" s="110" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z1" s="110" t="s">
+        <v>323</v>
+      </c>
+      <c r="AA1" s="110" t="s">
+        <v>324</v>
+      </c>
+      <c r="AB1" s="110" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>3</v>
@@ -28123,7 +28209,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0.03</v>
@@ -28133,11 +28219,74 @@
       </c>
       <c r="G2" s="111" t="n">
         <v>0.016</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0.682274557983333</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.72787227306</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0.49106682994</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0.6415070944</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1.84089048016</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>2.9371217298</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>0.0610567026182916</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>0.0835662684663543</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0.0905413542341182</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>0.181858939105416</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0.956447038228612</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>1.54745186194169</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>0.183745683176953</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>0.0865435526586513</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>0.124550106010302</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>0.253747085372654</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>0.195929442830894</v>
+      </c>
+      <c r="Y2" s="112" t="n">
+        <v>0.0432051810651043</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>0.308854599233992</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>0.076925939747246</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>0.231554540232771</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -28146,7 +28295,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.05</v>
@@ -28156,11 +28305,74 @@
       </c>
       <c r="G3" s="111" t="n">
         <v>0.0376</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.72671385258</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.774766858143478</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.641675627878261</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.758108764030435</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>3.00913251662609</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>3.90578349474783</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0.0597586842039105</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0.045310184139646</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0.121837738436168</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0.13815146998673</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>0.824761986096553</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>0.948257752303736</v>
+      </c>
+      <c r="T3" s="112" t="n">
+        <v>0.00230145837174289</v>
+      </c>
+      <c r="U3" s="112" t="n">
+        <v>0.00306538988910711</v>
+      </c>
+      <c r="V3" s="112" t="n">
+        <v>0.0012208268004514</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>0.484246737128615</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>0.321376005018267</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>0.0213830632219443</v>
+      </c>
+      <c r="Z3" s="112" t="n">
+        <v>0.0138110665772309</v>
+      </c>
+      <c r="AA3" s="112" t="n">
+        <v>0.0164501278382048</v>
+      </c>
+      <c r="AB3" s="112" t="n">
+        <v>0.0363617485471155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>742</v>
@@ -28169,7 +28381,7 @@
         <v>28</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>8.38</v>
@@ -28179,11 +28391,74 @@
       </c>
       <c r="G4" s="111" t="n">
         <v>8.18E-005</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.742206052780303</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.817507707365625</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.594632669009375</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.710522486290625</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>2.75642487478281</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>3.63750732494531</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0.18062687630405</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>0.406933453741526</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0.110071702807848</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.14749499211494</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0.865155675391224</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>1.19170797868159</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>0.0898977950102925</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>2.11180702693675E-006</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>5.32868978696258E-006</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0.270721364173735</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>0.169624094430809</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>0.261655450223721</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>0.12406019343742</v>
+      </c>
+      <c r="AA4" s="112" t="n">
+        <v>0.0983693110954592</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>0.214531514568973</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5855</v>
@@ -28192,7 +28467,7 @@
         <v>149</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>66.11</v>
@@ -28202,11 +28477,74 @@
       </c>
       <c r="G5" s="111" t="n">
         <v>7.42E-026</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.707370739166667</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.798174</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.74685686865</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.803329</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>3.8679107906</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>4.457434</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0.102525420625139</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0.048726</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0.16136065165</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.196621</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>1.1117865536</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0.959236</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0.205701317528004</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>0.403158729036529</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>0.335630370630132</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.439514337115215</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>0.276746854240925</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>0.195294082542879</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>0.277068831960179</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>0.176823299375759</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>0.197612305453449</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3</v>
@@ -28215,7 +28553,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.03</v>
@@ -28225,11 +28563,74 @@
       </c>
       <c r="G6" s="111" t="n">
         <v>0.016</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.756651914514286</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.807535661616667</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.73081372215</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.871562707066667</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>3.74401135896667</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>4.83615188383333</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0.0288904748251838</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0.0366006445613812</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>0.102488888594733</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.0823606405220116</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0.558079713473465</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0.442934580568129</v>
+      </c>
+      <c r="T6" s="112" t="n">
+        <v>0.0201683041219882</v>
+      </c>
+      <c r="U6" s="112" t="n">
+        <v>0.0234878062515265</v>
+      </c>
+      <c r="V6" s="112" t="n">
+        <v>0.00661479765279532</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0.284871827348097</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>0.0546595315668135</v>
+      </c>
+      <c r="Y6" s="112" t="n">
+        <v>0.00924684802459283</v>
+      </c>
+      <c r="Z6" s="112" t="n">
+        <v>0.00162944719918288</v>
+      </c>
+      <c r="AA6" s="112" t="n">
+        <v>0.0022573165449629</v>
+      </c>
+      <c r="AB6" s="112" t="n">
+        <v>0.00055527182474581</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>25</v>
@@ -28238,7 +28639,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0.28</v>
@@ -28248,11 +28649,74 @@
       </c>
       <c r="G7" s="111" t="n">
         <v>8.05E-013</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.703423055628571</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.714310222166667</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.6218845627</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.643401888883333</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>2.95305862611667</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>3.19613611116667</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.0698004023038643</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0.126262116249777</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0.137907467597558</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.24223597195659</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>1.01778481555915</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>1.63933707777937</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0.429128051672705</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>0.428730075354286</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>0.385045041808618</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0.355451876670106</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>0.187874993670404</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>0.269625840636711</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>0.343770121118318</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>0.21795927882829</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>0.334565730853791</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>201</v>
@@ -28261,7 +28725,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>2.27</v>
@@ -28271,11 +28735,74 @@
       </c>
       <c r="G8" s="111" t="n">
         <v>9.73E-021</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.7608665431375</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.807486709957143</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.738337850185714</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.851530248914286</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>3.68146968901429</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>4.70643825757143</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0.0250779396774854</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>0.0367571210379317</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>0.0742785105024933</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.0903976805719401</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.527106953806076</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>0.493309892643984</v>
+      </c>
+      <c r="T8" s="112" t="n">
+        <v>0.0150042432588113</v>
+      </c>
+      <c r="U8" s="112" t="n">
+        <v>0.0214645868344452</v>
+      </c>
+      <c r="V8" s="112" t="n">
+        <v>0.00471982542776034</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0.241344327918474</v>
+      </c>
+      <c r="X8" s="112" t="n">
+        <v>0.0454179494995398</v>
+      </c>
+      <c r="Y8" s="112" t="n">
+        <v>0.000937155989369291</v>
+      </c>
+      <c r="Z8" s="112" t="n">
+        <v>0.00177477337558013</v>
+      </c>
+      <c r="AA8" s="112" t="n">
+        <v>0.000966573826256753</v>
+      </c>
+      <c r="AB8" s="112" t="n">
+        <v>0.000522895944193788</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>281</v>
@@ -28284,7 +28811,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.17</v>
@@ -28294,11 +28821,74 @@
       </c>
       <c r="G9" s="111" t="n">
         <v>5.58E-021</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.733043844315385</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.738596187091667</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0.622988318675</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.788457806283334</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>2.99908575714167</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>4.37239526111667</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.0495854326855042</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0.205134030368362</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>0.136815220506997</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.131182925415896</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0.966690625197249</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>1.042314246604</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>0.464435447505477</v>
+      </c>
+      <c r="U9" s="112" t="n">
+        <v>0.00578534025863302</v>
+      </c>
+      <c r="V9" s="112" t="n">
+        <v>0.00325916952913185</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0.424325754553615</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>0.328519519896431</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>0.179572912473666</v>
+      </c>
+      <c r="Z9" s="112" t="n">
+        <v>0.0120712429581692</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>0.0931842824314924</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>0.00879446843228985</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2385</v>
@@ -28307,7 +28897,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>26.93</v>
@@ -28317,11 +28907,74 @@
       </c>
       <c r="G10" s="111" t="n">
         <v>0.014</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.719764826077778</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.777825163625</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.6207954484</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.76515071425</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>2.7660040072875</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>3.9082179316625</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0.0448882848185764</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>0.0484718394364012</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0.0956211998176618</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.117277857451975</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0.720419199173668</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>1.29243049322945</v>
+      </c>
+      <c r="T10" s="112" t="n">
+        <v>0.0189942172441517</v>
+      </c>
+      <c r="U10" s="112" t="n">
+        <v>0.0153581765672228</v>
+      </c>
+      <c r="V10" s="112" t="n">
+        <v>0.0326563824087389</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0.451524498741572</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>0.31616140576034</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>0.164953214697656</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>0.0529671976502482</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>0.270134828722458</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>0.205327802281984</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>4</v>
@@ -28330,7 +28983,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0.05</v>
@@ -28340,11 +28993,74 @@
       </c>
       <c r="G11" s="111" t="n">
         <v>0.0376</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.715788107</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.7268709007</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.5739637035</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.6476186505</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>2.6064939911</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>3.253945627</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0.066961067</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0.0915844563</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>0.1083826005</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.1505642065</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0.9976926609</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>1.448976516</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>0.456302202739292</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>0.337148081370666</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>0.347246029596194</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0.468778372810591</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>0.328974880479235</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>0.4569966991353</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>0.390860742967112</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <v>0.496317703339355</v>
+      </c>
+      <c r="AB11" s="0" t="n">
+        <v>0.424625870520953</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>17</v>
@@ -28353,7 +29069,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.19</v>
@@ -28363,11 +29079,74 @@
       </c>
       <c r="G12" s="111" t="n">
         <v>3.8E-006</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.72671385258</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.774766858143478</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.641675627878261</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.758108764030435</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>3.00913251662609</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>3.90578349474783</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0.0597586842039105</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>0.045310184139646</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>0.121837738436168</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.13815146998673</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0.824761986096553</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>0.948257752303736</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>0.00230145837174289</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>0.00306538988910711</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>0.0012208268004514</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>0.484246737128615</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>0.321376005018267</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>0.0213830632219443</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>0.0138110665772309</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <v>0.0164501278382048</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>0.0363617485471155</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2511</v>
@@ -28376,7 +29155,7 @@
         <v>71</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>28.35</v>
@@ -28386,11 +29165,74 @@
       </c>
       <c r="G13" s="111" t="n">
         <v>3.02E-010</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.791257704073684</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.932109532426316</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0.54761075108421</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0.650516935752632</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>2.55890536311579</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>3.55587414153158</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>0.318315143212357</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>0.729820778611272</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>0.0799176442554203</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>0.146959890707234</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0.694103546376028</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>1.26574919451194</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>0.225327672347045</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>0.00762058876485049</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>0.00375699517435092</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>0.206439343750321</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <v>0.168735943953952</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>0.0409196368223114</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>0.165369904802762</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>0.408803771097798</v>
+      </c>
+      <c r="AB13" s="0" t="n">
+        <v>0.430169976907256</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>15</v>
@@ -28399,7 +29241,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.17</v>
@@ -28409,11 +29251,74 @@
       </c>
       <c r="G14" s="111" t="n">
         <v>6.85E-005</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.735356914380952</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.773138426001527</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0.595595326259542</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0.678524846992366</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>2.63524447134809</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>3.46881111427939</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>0.15566688247474</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>0.297910298758851</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>0.141886277032494</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>0.160123151622929</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0.88890432072291</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>1.23431828039677</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>0.0976464856637999</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>9.64157231841923E-006</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>2.43531541751526E-009</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>0.280555466822856</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>0.412121081514774</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>0.224918360273747</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>0.338777522193158</v>
+      </c>
+      <c r="AA14" s="0" t="n">
+        <v>0.34901533897941</v>
+      </c>
+      <c r="AB14" s="0" t="n">
+        <v>0.403617748326356</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>98</v>
@@ -28422,7 +29327,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1.11</v>
@@ -28432,11 +29337,74 @@
       </c>
       <c r="G15" s="111" t="n">
         <v>4.82E-013</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0.6522113088</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0.7240788718</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0.443057178666667</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.5965131282</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>1.5694991125</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>2.51338702563333</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0.0398758771940997</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>0.0190112838952889</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>0.0289924589371274</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0.0788994969515443</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0.259241313347803</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>1.08470833276504</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>0.0531245042646534</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>0.0435703218698369</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>0.14015899484559</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>0.215735459810492</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <v>0.07466151249922</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <v>0.00837102279571253</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>0.098129291190166</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <v>0.0115806050281293</v>
+      </c>
+      <c r="AB15" s="0" t="n">
+        <v>0.129016079065395</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>124</v>
@@ -28445,7 +29413,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1.4</v>
@@ -28455,11 +29423,74 @@
       </c>
       <c r="G16" s="111" t="n">
         <v>1.76E-012</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0.715788107</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0.7268709007</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0.5739637035</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0.6476186505</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>2.6064939911</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>3.253945627</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>0.066961067</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0.0915844563</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>0.1083826005</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0.1505642065</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0.9976926609</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>1.448976516</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>0.456302202739292</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>0.337148081370666</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>0.347246029596194</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>0.468778372810591</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>0.328974880479235</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>0.4569966991353</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>0.390860742967112</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <v>0.496317703339355</v>
+      </c>
+      <c r="AB16" s="0" t="n">
+        <v>0.424625870520953</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>27</v>
@@ -28468,7 +29499,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.3</v>
@@ -28478,11 +29509,74 @@
       </c>
       <c r="G17" s="111" t="n">
         <v>0.00208</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0.7608665431375</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0.807486709957143</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0.738337850185714</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0.851530248914286</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>3.68146968901429</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>4.70643825757143</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>0.0250779396774854</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0.0367571210379317</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0.0742785105024933</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0.0903976805719401</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>0.527106953806076</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>0.493309892643984</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>0.0150042432588113</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>0.0214645868344452</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>0.00471982542776034</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>0.241344327918474</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <v>0.0454179494995398</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <v>0.000937155989369291</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>0.00177477337558013</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>0.000966573826256753</v>
+      </c>
+      <c r="AB17" s="0" t="n">
+        <v>0.000522895944193788</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -28491,7 +29585,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.34</v>
@@ -28501,11 +29595,74 @@
       </c>
       <c r="G18" s="111" t="n">
         <v>0.00381</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.72760073541</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0.7834485416625</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0.6505898117375</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.7753187083375</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>3.1325877439125</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>4.3041567290875</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0.064660965654419</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>0.0598062393464362</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>0.118858891277758</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0.170846591430589</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>0.842338878640247</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>1.00044483894632</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>0.0497008222173976</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>0.0669422809019822</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>0.0195097728998582</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>0.483760389927663</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <v>0.266263164738276</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <v>0.0829117450680221</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <v>0.0938148871046756</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <v>0.0605017995356827</v>
+      </c>
+      <c r="AB18" s="0" t="n">
+        <v>0.0314614528839145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>27</v>
@@ -28514,7 +29671,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0.3</v>
@@ -28524,11 +29681,74 @@
       </c>
       <c r="G19" s="111" t="n">
         <v>0.00208</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.715788107</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0.7268709007</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0.5739637035</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.6476186505</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>2.6064939911</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>3.253945627</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0.066961067</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0.0915844563</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>0.1083826005</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0.1505642065</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>0.9976926609</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>1.448976516</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>0.456302202739292</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>0.337148081370666</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <v>0.347246029596194</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>0.468778372810591</v>
+      </c>
+      <c r="X19" s="0" t="n">
+        <v>0.328974880479235</v>
+      </c>
+      <c r="Y19" s="0" t="n">
+        <v>0.4569966991353</v>
+      </c>
+      <c r="Z19" s="0" t="n">
+        <v>0.390860742967112</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <v>0.496317703339355</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <v>0.424625870520953</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>10703</v>
@@ -28537,7 +29757,7 @@
         <v>155</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>120.84</v>
@@ -28547,11 +29767,74 @@
       </c>
       <c r="G20" s="111" t="n">
         <v>0.0119</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.7608665431375</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0.807486709957143</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0.738337850185714</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.851530248914286</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>3.68146968901429</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>4.70643825757143</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0.0250779396774854</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>0.0367571210379317</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>0.0742785105024933</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>0.0903976805719401</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>0.527106953806076</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>0.493309892643984</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>0.0150042432588113</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>0.0214645868344452</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>0.00471982542776034</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>0.241344327918474</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <v>0.0454179494995398</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <v>0.000937155989369291</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>0.00177477337558013</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>0.000966573826256753</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <v>0.000522895944193788</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>50</v>
@@ -28560,7 +29843,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0.56</v>
@@ -28570,11 +29853,74 @@
       </c>
       <c r="G21" s="111" t="n">
         <v>2.17E-005</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0.703309679164706</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0.73837687619</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0.593487981693333</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.71213051844</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>2.65307146546667</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>3.67997978261333</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0.0571406464956032</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>0.13701392854744</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>0.125325542735567</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0.146796253104586</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <v>0.96257796536601</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <v>1.33362091485765</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>0.101033957620184</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>0.00107985673623553</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <v>0.000940418415111172</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>0.186219976492803</v>
+      </c>
+      <c r="X21" s="0" t="n">
+        <v>0.171435490079328</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <v>0.355666890507518</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <v>0.183904557899388</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <v>0.384089311959522</v>
+      </c>
+      <c r="AB21" s="0" t="n">
+        <v>0.24710683082652</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>138</v>
@@ -28583,7 +29929,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1.56</v>
@@ -28593,11 +29939,74 @@
       </c>
       <c r="G22" s="111" t="n">
         <v>2.51E-006</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.682274557983333</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0.72787227306</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0.49106682994</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.6415070944</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>1.84089048016</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>2.9371217298</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0.0610567026182916</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>0.0835662684663543</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>0.0905413542341182</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>0.181858939105416</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>0.956447038228612</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <v>1.54745186194169</v>
+      </c>
+      <c r="T22" s="0" t="n">
+        <v>0.183745683176953</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>0.0865435526586513</v>
+      </c>
+      <c r="V22" s="0" t="n">
+        <v>0.124550106010302</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>0.253747085372654</v>
+      </c>
+      <c r="X22" s="0" t="n">
+        <v>0.195929442830894</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <v>0.0432051810651043</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <v>0.308854599233992</v>
+      </c>
+      <c r="AA22" s="0" t="n">
+        <v>0.076925939747246</v>
+      </c>
+      <c r="AB22" s="0" t="n">
+        <v>0.231554540232771</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>45</v>
@@ -28606,7 +30015,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>0.51</v>
@@ -28616,11 +30025,74 @@
       </c>
       <c r="G23" s="111" t="n">
         <v>0.000162</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.715788107</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0.7268709007</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0.5739637035</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.6476186505</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>2.6064939911</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>3.253945627</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.066961067</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>0.0915844563</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>0.1083826005</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>0.1505642065</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>0.9976926609</v>
+      </c>
+      <c r="S23" s="0" t="n">
+        <v>1.448976516</v>
+      </c>
+      <c r="T23" s="0" t="n">
+        <v>0.456302202739292</v>
+      </c>
+      <c r="U23" s="0" t="n">
+        <v>0.337148081370666</v>
+      </c>
+      <c r="V23" s="0" t="n">
+        <v>0.347246029596194</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>0.468778372810591</v>
+      </c>
+      <c r="X23" s="0" t="n">
+        <v>0.328974880479235</v>
+      </c>
+      <c r="Y23" s="0" t="n">
+        <v>0.4569966991353</v>
+      </c>
+      <c r="Z23" s="0" t="n">
+        <v>0.390860742967112</v>
+      </c>
+      <c r="AA23" s="0" t="n">
+        <v>0.496317703339355</v>
+      </c>
+      <c r="AB23" s="0" t="n">
+        <v>0.424625870520953</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>45</v>
@@ -28629,7 +30101,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0.51</v>
@@ -28639,11 +30111,74 @@
       </c>
       <c r="G24" s="111" t="n">
         <v>0.000162</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0.65833170178</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>0.73736684616</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0.4911114066</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.65929815384</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>1.8982774046</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>2.98679063076</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0.0494667305728679</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>0.0411658469713016</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>0.0927033811586141</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>0.132842839879895</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>0.61371494428664</v>
+      </c>
+      <c r="S24" s="0" t="n">
+        <v>1.17020045671686</v>
+      </c>
+      <c r="T24" s="0" t="n">
+        <v>0.0257894552276943</v>
+      </c>
+      <c r="U24" s="0" t="n">
+        <v>0.040497669964747</v>
+      </c>
+      <c r="V24" s="0" t="n">
+        <v>0.0696357794549139</v>
+      </c>
+      <c r="W24" s="0" t="n">
+        <v>0.161152305195632</v>
+      </c>
+      <c r="X24" s="0" t="n">
+        <v>0.143395897463467</v>
+      </c>
+      <c r="Y24" s="0" t="n">
+        <v>0.0457681169656196</v>
+      </c>
+      <c r="Z24" s="0" t="n">
+        <v>0.341522044854687</v>
+      </c>
+      <c r="AA24" s="0" t="n">
+        <v>0.0333343834446593</v>
+      </c>
+      <c r="AB24" s="0" t="n">
+        <v>0.192937375485184</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>59</v>
@@ -28652,7 +30187,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>0.67</v>
@@ -28662,11 +30197,74 @@
       </c>
       <c r="G25" s="111" t="n">
         <v>0.00124</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0.7256711127625</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>0.6994576303</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>0.623092312471429</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0.782358156057143</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>2.99519219892857</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>4.38413670948571</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0.0471449858352203</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>0.258220074161351</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>0.117941190124005</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>0.121480024254411</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>0.831722435352437</v>
+      </c>
+      <c r="S25" s="0" t="n">
+        <v>1.00360053234807</v>
+      </c>
+      <c r="T25" s="0" t="n">
+        <v>0.400030002241833</v>
+      </c>
+      <c r="U25" s="0" t="n">
+        <v>0.023621913284247</v>
+      </c>
+      <c r="V25" s="0" t="n">
+        <v>0.0151911888865478</v>
+      </c>
+      <c r="W25" s="0" t="n">
+        <v>0.499284423693706</v>
+      </c>
+      <c r="X25" s="0" t="n">
+        <v>0.261328314668403</v>
+      </c>
+      <c r="Y25" s="0" t="n">
+        <v>0.213013112282739</v>
+      </c>
+      <c r="Z25" s="0" t="n">
+        <v>0.043108973490282</v>
+      </c>
+      <c r="AA25" s="0" t="n">
+        <v>0.129977492468829</v>
+      </c>
+      <c r="AB25" s="0" t="n">
+        <v>0.0317248197946598</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>100</v>
@@ -28675,7 +30273,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1.13</v>
@@ -28685,11 +30283,74 @@
       </c>
       <c r="G26" s="111" t="n">
         <v>0.00682</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.728000828183333</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0.7769584057</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>0.555800795733333</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.717236269366667</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>2.6398149652</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>4.1194148355</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0.0336836148769944</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>0.0396139006854232</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>0.0745680179615647</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0.104608398408703</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>0.587483718394249</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <v>0.77596773852331</v>
+      </c>
+      <c r="T26" s="0" t="n">
+        <v>0.034615613914527</v>
+      </c>
+      <c r="U26" s="0" t="n">
+        <v>0.0137638003627917</v>
+      </c>
+      <c r="V26" s="0" t="n">
+        <v>0.00682924963676898</v>
+      </c>
+      <c r="W26" s="0" t="n">
+        <v>0.482448586867419</v>
+      </c>
+      <c r="X26" s="0" t="n">
+        <v>0.326717349579811</v>
+      </c>
+      <c r="Y26" s="0" t="n">
+        <v>0.20222778000526</v>
+      </c>
+      <c r="Z26" s="0" t="n">
+        <v>0.253359745830798</v>
+      </c>
+      <c r="AA26" s="0" t="n">
+        <v>0.436311368827669</v>
+      </c>
+      <c r="AB26" s="0" t="n">
+        <v>0.0589689790585951</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>45</v>
@@ -28698,7 +30359,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0.51</v>
@@ -28708,11 +30369,74 @@
       </c>
       <c r="G27" s="111" t="n">
         <v>0.000162</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0.7608665431375</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0.807486709957143</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>0.738337850185714</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0.851530248914286</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>3.68146968901429</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>4.70643825757143</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>0.0250779396774854</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>0.0367571210379317</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>0.0742785105024933</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>0.0903976805719401</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>0.527106953806076</v>
+      </c>
+      <c r="S27" s="0" t="n">
+        <v>0.493309892643984</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <v>0.0150042432588113</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <v>0.0214645868344452</v>
+      </c>
+      <c r="V27" s="0" t="n">
+        <v>0.00471982542776034</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <v>0.241344327918474</v>
+      </c>
+      <c r="X27" s="0" t="n">
+        <v>0.0454179494995398</v>
+      </c>
+      <c r="Y27" s="0" t="n">
+        <v>0.000937155989369291</v>
+      </c>
+      <c r="Z27" s="0" t="n">
+        <v>0.00177477337558013</v>
+      </c>
+      <c r="AA27" s="0" t="n">
+        <v>0.000966573826256753</v>
+      </c>
+      <c r="AB27" s="0" t="n">
+        <v>0.000522895944193788</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>68</v>
@@ -28721,7 +30445,7 @@
         <v>7</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>0.77</v>
@@ -28731,11 +30455,74 @@
       </c>
       <c r="G28" s="111" t="n">
         <v>0.0382</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>0.7256604785</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0.778589891603846</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0.646984945680769</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>0.782284950669231</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>3.13142583525</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>4.20480889565385</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>0.0640504287309133</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>0.0556145730074413</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>0.131037234101697</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <v>0.130282279406503</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <v>0.968802880835695</v>
+      </c>
+      <c r="S28" s="0" t="n">
+        <v>1.07636170867953</v>
+      </c>
+      <c r="T28" s="0" t="n">
+        <v>0.00164933044573486</v>
+      </c>
+      <c r="U28" s="0" t="n">
+        <v>0.000489393529038395</v>
+      </c>
+      <c r="V28" s="0" t="n">
+        <v>0.000435497994068349</v>
+      </c>
+      <c r="W28" s="0" t="n">
+        <v>0.498809874815674</v>
+      </c>
+      <c r="X28" s="0" t="n">
+        <v>0.25881636961641</v>
+      </c>
+      <c r="Y28" s="0" t="n">
+        <v>0.0142282217427392</v>
+      </c>
+      <c r="Z28" s="0" t="n">
+        <v>0.000896028836528032</v>
+      </c>
+      <c r="AA28" s="0" t="n">
+        <v>0.00618029154034848</v>
+      </c>
+      <c r="AB28" s="0" t="n">
+        <v>0.00236376533779959</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>68</v>
@@ -28744,7 +30531,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>0.77</v>
@@ -28754,11 +30541,74 @@
       </c>
       <c r="G29" s="111" t="n">
         <v>0.0382</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>0.72671385258</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>0.774766858143478</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>0.641675627878261</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>0.758108764030435</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>3.00913251662609</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>3.90578349474783</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>0.0597586842039105</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>0.045310184139646</v>
+      </c>
+      <c r="P29" s="0" t="n">
+        <v>0.121837738436168</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <v>0.13815146998673</v>
+      </c>
+      <c r="R29" s="0" t="n">
+        <v>0.824761986096553</v>
+      </c>
+      <c r="S29" s="0" t="n">
+        <v>0.948257752303736</v>
+      </c>
+      <c r="T29" s="0" t="n">
+        <v>0.00230145837174289</v>
+      </c>
+      <c r="U29" s="0" t="n">
+        <v>0.00306538988910711</v>
+      </c>
+      <c r="V29" s="0" t="n">
+        <v>0.0012208268004514</v>
+      </c>
+      <c r="W29" s="0" t="n">
+        <v>0.484246737128615</v>
+      </c>
+      <c r="X29" s="0" t="n">
+        <v>0.321376005018267</v>
+      </c>
+      <c r="Y29" s="0" t="n">
+        <v>0.0213830632219443</v>
+      </c>
+      <c r="Z29" s="0" t="n">
+        <v>0.0138110665772309</v>
+      </c>
+      <c r="AA29" s="0" t="n">
+        <v>0.0164501278382048</v>
+      </c>
+      <c r="AB29" s="0" t="n">
+        <v>0.0363617485471155</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>70</v>
@@ -28767,7 +30617,7 @@
         <v>7</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>0.79</v>
@@ -28777,11 +30627,74 @@
       </c>
       <c r="G30" s="111" t="n">
         <v>0.046</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>0.734206069666667</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>0.7763819445</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>0.6073189945</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>0.724519752333333</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>3.10877319283333</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>3.92826366266667</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>0.038016622367566</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>0.0329291663570538</v>
+      </c>
+      <c r="P30" s="0" t="n">
+        <v>0.0744194896494437</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <v>0.0822106127529732</v>
+      </c>
+      <c r="R30" s="0" t="n">
+        <v>0.669171644538532</v>
+      </c>
+      <c r="S30" s="0" t="n">
+        <v>0.51796244304704</v>
+      </c>
+      <c r="T30" s="0" t="n">
+        <v>0.0475745429161774</v>
+      </c>
+      <c r="U30" s="0" t="n">
+        <v>0.0244520478169225</v>
+      </c>
+      <c r="V30" s="0" t="n">
+        <v>0.0318916697227677</v>
+      </c>
+      <c r="W30" s="0" t="n">
+        <v>0.438365228788087</v>
+      </c>
+      <c r="X30" s="0" t="n">
+        <v>0.32112328598208</v>
+      </c>
+      <c r="Y30" s="0" t="n">
+        <v>0.249438359626976</v>
+      </c>
+      <c r="Z30" s="0" t="n">
+        <v>0.160500722853111</v>
+      </c>
+      <c r="AA30" s="0" t="n">
+        <v>0.063205833240996</v>
+      </c>
+      <c r="AB30" s="0" t="n">
+        <v>0.0595784512032944</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>121</v>
@@ -28790,7 +30703,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1.37</v>
@@ -28800,11 +30713,74 @@
       </c>
       <c r="G31" s="111" t="n">
         <v>0.0309</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>0.752307667122222</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>0.7948612878375</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>0.7176518414125</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>0.815313551175</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>3.4955945510125</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>4.22591555875</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>0.0338387323938008</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>0.0479375551057486</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>0.0884477907859709</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>0.12779599930029</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>0.696389611960977</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>1.35249760350482</v>
+      </c>
+      <c r="T31" s="0" t="n">
+        <v>0.03747477735645</v>
+      </c>
+      <c r="U31" s="0" t="n">
+        <v>0.0593790230017578</v>
+      </c>
+      <c r="V31" s="0" t="n">
+        <v>0.108324104139791</v>
+      </c>
+      <c r="W31" s="0" t="n">
+        <v>0.285245959253038</v>
+      </c>
+      <c r="X31" s="0" t="n">
+        <v>0.12439581154791</v>
+      </c>
+      <c r="Y31" s="0" t="n">
+        <v>0.002204787362543</v>
+      </c>
+      <c r="Z31" s="0" t="n">
+        <v>0.013409528959383</v>
+      </c>
+      <c r="AA31" s="0" t="n">
+        <v>0.00462423847193306</v>
+      </c>
+      <c r="AB31" s="0" t="n">
+        <v>0.0896783418293576</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>135</v>
@@ -28813,7 +30789,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1.52</v>
@@ -28823,11 +30799,74 @@
       </c>
       <c r="G32" s="111" t="n">
         <v>0.0105</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>0.6985438753</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0.767515</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>0.66109628845</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>0.69389666665</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>2.97399620675</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>3.81237</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>0.0599229156768504</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>0.066505</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>0.07045371155</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <v>0.12279333335</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <v>0.70099974525</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <v>1.96515</v>
+      </c>
+      <c r="T32" s="0" t="n">
+        <v>0.223592109445728</v>
+      </c>
+      <c r="U32" s="0" t="n">
+        <v>0.399211519086324</v>
+      </c>
+      <c r="V32" s="0" t="n">
+        <v>0.335511847611797</v>
+      </c>
+      <c r="W32" s="0" t="n">
+        <v>0.400457401952483</v>
+      </c>
+      <c r="X32" s="0" t="n">
+        <v>0.493208320244024</v>
+      </c>
+      <c r="Y32" s="0" t="n">
+        <v>0.185264263925819</v>
+      </c>
+      <c r="Z32" s="0" t="n">
+        <v>0.4706395608528</v>
+      </c>
+      <c r="AA32" s="0" t="n">
+        <v>0.294485927887416</v>
+      </c>
+      <c r="AB32" s="0" t="n">
+        <v>0.4301700738135</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>786</v>
@@ -28836,7 +30875,7 @@
         <v>26</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>8.87</v>
@@ -28846,11 +30885,74 @@
       </c>
       <c r="G33" s="111" t="n">
         <v>0.0031</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>0.756651914514286</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0.807535661616667</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>0.73081372215</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>0.871562707066667</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>3.74401135896667</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>4.83615188383333</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>0.0288904748251838</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>0.0366006445613812</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <v>0.102488888594733</v>
+      </c>
+      <c r="Q33" s="0" t="n">
+        <v>0.0823606405220116</v>
+      </c>
+      <c r="R33" s="0" t="n">
+        <v>0.558079713473465</v>
+      </c>
+      <c r="S33" s="0" t="n">
+        <v>0.442934580568129</v>
+      </c>
+      <c r="T33" s="0" t="n">
+        <v>0.0201683041219882</v>
+      </c>
+      <c r="U33" s="0" t="n">
+        <v>0.0234878062515265</v>
+      </c>
+      <c r="V33" s="0" t="n">
+        <v>0.00661479765279532</v>
+      </c>
+      <c r="W33" s="0" t="n">
+        <v>0.284871827348097</v>
+      </c>
+      <c r="X33" s="0" t="n">
+        <v>0.0546595315668135</v>
+      </c>
+      <c r="Y33" s="0" t="n">
+        <v>0.00924684802459283</v>
+      </c>
+      <c r="Z33" s="0" t="n">
+        <v>0.00162944719918288</v>
+      </c>
+      <c r="AA33" s="0" t="n">
+        <v>0.0022573165449629</v>
+      </c>
+      <c r="AB33" s="0" t="n">
+        <v>0.00055527182474581</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>826</v>
@@ -28859,7 +30961,7 @@
         <v>26</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>9.33</v>
@@ -28869,11 +30971,74 @@
       </c>
       <c r="G34" s="111" t="n">
         <v>0.0076</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>0.707370739166667</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>0.798174</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>0.74685686865</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>0.803329</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>3.8679107906</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>4.457434</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>0.102525420625139</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>0.048726</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <v>0.16136065165</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <v>0.196621</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <v>1.1117865536</v>
+      </c>
+      <c r="S34" s="0" t="n">
+        <v>0.959236</v>
+      </c>
+      <c r="T34" s="0" t="n">
+        <v>0.205701317528004</v>
+      </c>
+      <c r="U34" s="0" t="n">
+        <v>0.403158729036529</v>
+      </c>
+      <c r="V34" s="0" t="n">
+        <v>0.335630370630132</v>
+      </c>
+      <c r="W34" s="0" t="n">
+        <v>0.439514337115215</v>
+      </c>
+      <c r="X34" s="0" t="n">
+        <v>0.276746854240925</v>
+      </c>
+      <c r="Y34" s="0" t="n">
+        <v>0.195294082542879</v>
+      </c>
+      <c r="Z34" s="0" t="n">
+        <v>0.277068831960179</v>
+      </c>
+      <c r="AA34" s="0" t="n">
+        <v>0.176823299375759</v>
+      </c>
+      <c r="AB34" s="0" t="n">
+        <v>0.197612305453449</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>829</v>
@@ -28882,7 +31047,7 @@
         <v>26</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>9.36</v>
@@ -28892,11 +31057,74 @@
       </c>
       <c r="G35" s="111" t="n">
         <v>0.81</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>0.666578984509091</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>0.727525937281818</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>0.526902588</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>0.635995382827273</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>2.02204495674545</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <v>3.03654765331818</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>0.018607443935088</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>0.0479255011036399</v>
+      </c>
+      <c r="P35" s="0" t="n">
+        <v>0.0354366892985672</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <v>0.128750825610382</v>
+      </c>
+      <c r="R35" s="0" t="n">
+        <v>0.236104793615077</v>
+      </c>
+      <c r="S35" s="0" t="n">
+        <v>1.09601883945834</v>
+      </c>
+      <c r="T35" s="0" t="n">
+        <v>0.00140598574383824</v>
+      </c>
+      <c r="U35" s="0" t="n">
+        <v>0.0109766070540604</v>
+      </c>
+      <c r="V35" s="0" t="n">
+        <v>0.00665922307068617</v>
+      </c>
+      <c r="W35" s="0" t="n">
+        <v>0.0744895510235045</v>
+      </c>
+      <c r="X35" s="0" t="n">
+        <v>0.0451471367601304</v>
+      </c>
+      <c r="Y35" s="0" t="n">
+        <v>0.000754239349618366</v>
+      </c>
+      <c r="Z35" s="0" t="n">
+        <v>0.121840087422445</v>
+      </c>
+      <c r="AA35" s="0" t="n">
+        <v>3.82216046577308E-005</v>
+      </c>
+      <c r="AB35" s="0" t="n">
+        <v>0.10084327189652</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>832</v>
@@ -28905,7 +31133,7 @@
         <v>26</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>9.39</v>
@@ -28915,11 +31143,74 @@
       </c>
       <c r="G36" s="111" t="n">
         <v>0.00864</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>0.716912442688889</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>0.760405548116667</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>0.550899001144444</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>0.651132807183333</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>2.58276274945556</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <v>3.52993485772778</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>0.0440060343463198</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>0.0454585861906163</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <v>0.080846858713981</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <v>0.150963067645186</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <v>0.705500496840907</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <v>1.29550903682277</v>
+      </c>
+      <c r="T36" s="0" t="n">
+        <v>0.00480994535508155</v>
+      </c>
+      <c r="U36" s="0" t="n">
+        <v>0.0118732516289201</v>
+      </c>
+      <c r="V36" s="0" t="n">
+        <v>0.00721438134306729</v>
+      </c>
+      <c r="W36" s="0" t="n">
+        <v>0.39145427884226</v>
+      </c>
+      <c r="X36" s="0" t="n">
+        <v>0.37280194582609</v>
+      </c>
+      <c r="Y36" s="0" t="n">
+        <v>0.0613241035908389</v>
+      </c>
+      <c r="Z36" s="0" t="n">
+        <v>0.181478513461629</v>
+      </c>
+      <c r="AA36" s="0" t="n">
+        <v>0.465137998221375</v>
+      </c>
+      <c r="AB36" s="0" t="n">
+        <v>0.465325212673824</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1400</v>
@@ -28928,21 +31219,84 @@
         <v>2</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>15.81</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G37" s="111" t="n">
         <v>0.0323</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>0.701110926294</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>0.738530861780435</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>0.580043654778261</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>0.693370743323913</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>2.57911609071522</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>3.47638581487391</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>0.0576963153993898</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <v>0.116244344026847</v>
+      </c>
+      <c r="P37" s="0" t="n">
+        <v>0.119965734607753</v>
+      </c>
+      <c r="Q37" s="0" t="n">
+        <v>0.150859859726409</v>
+      </c>
+      <c r="R37" s="0" t="n">
+        <v>0.933579817295164</v>
+      </c>
+      <c r="S37" s="0" t="n">
+        <v>1.28185621229861</v>
+      </c>
+      <c r="T37" s="0" t="n">
+        <v>0.0274291713601523</v>
+      </c>
+      <c r="U37" s="0" t="n">
+        <v>0.000121154911651731</v>
+      </c>
+      <c r="V37" s="0" t="n">
+        <v>0.000192562465117884</v>
+      </c>
+      <c r="W37" s="0" t="n">
+        <v>0.113381018460758</v>
+      </c>
+      <c r="X37" s="0" t="n">
+        <v>0.112677720644288</v>
+      </c>
+      <c r="Y37" s="0" t="n">
+        <v>0.410889639516655</v>
+      </c>
+      <c r="Z37" s="0" t="n">
+        <v>0.379872657961629</v>
+      </c>
+      <c r="AA37" s="0" t="n">
+        <v>0.448741281929954</v>
+      </c>
+      <c r="AB37" s="0" t="n">
+        <v>0.450848225132026</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1650</v>
@@ -28951,21 +31305,84 @@
         <v>2</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>18.63</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G38" s="111" t="n">
         <v>0.00251</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>0.701344814989655</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>0.729270199023077</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>0.598157292211538</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>0.698465982815385</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>2.64959930576538</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <v>3.54245297566538</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>0.0594758168577633</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <v>0.146838860392767</v>
+      </c>
+      <c r="P38" s="0" t="n">
+        <v>0.125312310110894</v>
+      </c>
+      <c r="Q38" s="0" t="n">
+        <v>0.157827276576237</v>
+      </c>
+      <c r="R38" s="0" t="n">
+        <v>0.976520666285477</v>
+      </c>
+      <c r="S38" s="0" t="n">
+        <v>1.48267482865136</v>
+      </c>
+      <c r="T38" s="0" t="n">
+        <v>0.186945165140469</v>
+      </c>
+      <c r="U38" s="0" t="n">
+        <v>0.00887793236768798</v>
+      </c>
+      <c r="V38" s="0" t="n">
+        <v>0.00836392795088337</v>
+      </c>
+      <c r="W38" s="0" t="n">
+        <v>0.185601924917931</v>
+      </c>
+      <c r="X38" s="0" t="n">
+        <v>0.131165040194036</v>
+      </c>
+      <c r="Y38" s="0" t="n">
+        <v>0.299964297887121</v>
+      </c>
+      <c r="Z38" s="0" t="n">
+        <v>0.350859970031728</v>
+      </c>
+      <c r="AA38" s="0" t="n">
+        <v>0.399440179946656</v>
+      </c>
+      <c r="AB38" s="0" t="n">
+        <v>0.447296644797842</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1650</v>
@@ -28974,21 +31391,84 @@
         <v>2</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>18.63</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G39" s="111" t="n">
         <v>0.00251</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>0.724145206769504</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>0.781829476469343</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>0.595802409991971</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>0.712583173364963</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>2.74508762612993</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <v>3.66578441301095</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>0.131398011563109</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <v>0.28929573948835</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <v>0.110456023812273</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>0.143906830998774</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <v>0.867527989636107</v>
+      </c>
+      <c r="S39" s="0" t="n">
+        <v>1.21300001640235</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <v>0.0174809263669244</v>
+      </c>
+      <c r="U39" s="0" t="n">
+        <v>3.08398367135938E-012</v>
+      </c>
+      <c r="V39" s="0" t="n">
+        <v>1.6126053371274E-011</v>
+      </c>
+      <c r="W39" s="0" t="n">
+        <v>0.462752934548897</v>
+      </c>
+      <c r="X39" s="0" t="n">
+        <v>0.297688494983027</v>
+      </c>
+      <c r="Y39" s="0" t="n">
+        <v>0.179193419184031</v>
+      </c>
+      <c r="Z39" s="0" t="n">
+        <v>0.0497956893052248</v>
+      </c>
+      <c r="AA39" s="0" t="n">
+        <v>0.0566914330366003</v>
+      </c>
+      <c r="AB39" s="0" t="n">
+        <v>0.109138285147727</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1741</v>
@@ -28997,21 +31477,84 @@
         <v>2</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>19.66</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G40" s="111" t="n">
         <v>0.000785</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>0.671721235766667</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0.731028055566667</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>0.5505112031</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>0.665740555566667</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>1.9766137795</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>2.98513583333333</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>0.00588056752241992</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>0.0702245942590828</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <v>0.0136578436566584</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <v>0.182658758633302</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <v>0.260733164251127</v>
+      </c>
+      <c r="S40" s="0" t="n">
+        <v>1.5705579746765</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <v>0.141138063384103</v>
+      </c>
+      <c r="U40" s="0" t="n">
+        <v>0.194835534633523</v>
+      </c>
+      <c r="V40" s="0" t="n">
+        <v>0.193506352201053</v>
+      </c>
+      <c r="W40" s="0" t="n">
+        <v>0.265028728701297</v>
+      </c>
+      <c r="X40" s="0" t="n">
+        <v>0.249148623739803</v>
+      </c>
+      <c r="Y40" s="0" t="n">
+        <v>0.0468778264018556</v>
+      </c>
+      <c r="Z40" s="0" t="n">
+        <v>0.433648024500399</v>
+      </c>
+      <c r="AA40" s="0" t="n">
+        <v>0.0302088252903529</v>
+      </c>
+      <c r="AB40" s="0" t="n">
+        <v>0.313743907697566</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>2466</v>
@@ -29020,21 +31563,84 @@
         <v>3</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>27.84</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G41" s="111" t="n">
         <v>1.98E-006</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>0.72671385258</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>0.774766858143478</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>0.641675627878261</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>0.758108764030435</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>3.00913251662609</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>3.90578349474783</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>0.0597586842039105</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>0.045310184139646</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <v>0.121837738436168</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>0.13815146998673</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <v>0.824761986096553</v>
+      </c>
+      <c r="S41" s="0" t="n">
+        <v>0.948257752303736</v>
+      </c>
+      <c r="T41" s="0" t="n">
+        <v>0.00230145837174289</v>
+      </c>
+      <c r="U41" s="0" t="n">
+        <v>0.00306538988910711</v>
+      </c>
+      <c r="V41" s="0" t="n">
+        <v>0.0012208268004514</v>
+      </c>
+      <c r="W41" s="0" t="n">
+        <v>0.484246737128615</v>
+      </c>
+      <c r="X41" s="0" t="n">
+        <v>0.321376005018267</v>
+      </c>
+      <c r="Y41" s="0" t="n">
+        <v>0.0213830632219443</v>
+      </c>
+      <c r="Z41" s="0" t="n">
+        <v>0.0138110665772309</v>
+      </c>
+      <c r="AA41" s="0" t="n">
+        <v>0.0164501278382048</v>
+      </c>
+      <c r="AB41" s="0" t="n">
+        <v>0.0363617485471155</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>3970</v>
@@ -29043,16 +31649,79 @@
         <v>7</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>44.82</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G42" s="111" t="n">
         <v>2.15E-008</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>0.6935956726</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0.7297418008</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>0.5045152096</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>0.568642697</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>2.0949556688</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>2.762885238</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>0.0359611309649168</v>
+      </c>
+      <c r="O42" s="0" t="n">
+        <v>0.0514770299501928</v>
+      </c>
+      <c r="P42" s="0" t="n">
+        <v>0.0817186570153809</v>
+      </c>
+      <c r="Q42" s="0" t="n">
+        <v>0.164167219467386</v>
+      </c>
+      <c r="R42" s="0" t="n">
+        <v>0.44127019044544</v>
+      </c>
+      <c r="S42" s="0" t="n">
+        <v>1.14132668946459</v>
+      </c>
+      <c r="T42" s="0" t="n">
+        <v>0.133737436219044</v>
+      </c>
+      <c r="U42" s="0" t="n">
+        <v>0.238973014987432</v>
+      </c>
+      <c r="V42" s="0" t="n">
+        <v>0.144643763271825</v>
+      </c>
+      <c r="W42" s="0" t="n">
+        <v>0.304256438343468</v>
+      </c>
+      <c r="X42" s="0" t="n">
+        <v>0.125856851469261</v>
+      </c>
+      <c r="Y42" s="0" t="n">
+        <v>0.0497095369423484</v>
+      </c>
+      <c r="Z42" s="0" t="n">
+        <v>0.0946430566906391</v>
+      </c>
+      <c r="AA42" s="0" t="n">
+        <v>0.0349209551303314</v>
+      </c>
+      <c r="AB42" s="0" t="n">
+        <v>0.113033646518237</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>